<commit_message>
moved supplementary files to correct column; populated geo_series column
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/current/filled/glioblastoma_1000cells.xlsx
+++ b/examples/spreadsheets/current/filled/glioblastoma_1000cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/Google Drive/metadata-schema/examples/spreadsheets/current/filled/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rolando/development/hca/metadata-schema/examples/spreadsheets/current/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B59412EC-B460-EE4D-8E34-3DB697590A87}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E93754C4-E89F-5C47-A681-2E7EF2814510}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25580" yWindow="460" windowWidth="25600" windowHeight="27480" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-10800" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20154" uniqueCount="3788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20155" uniqueCount="3789">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -11399,6 +11399,9 @@
   </si>
   <si>
     <t>EFO:0008442</t>
+  </si>
+  <si>
+    <t>GSE84nnn</t>
   </si>
 </sst>
 </file>
@@ -11870,8 +11873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11879,7 +11882,7 @@
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" customWidth="1"/>
@@ -11993,14 +11996,21 @@
       <c r="C6" s="7" t="s">
         <v>657</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>658</v>
+      <c r="D6" s="4"/>
+      <c r="E6" t="s">
+        <v>3788</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>659</v>
       </c>
+      <c r="G6" s="4" t="s">
+        <v>658</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G6" r:id="rId1" xr:uid="{DAB3418F-8794-9D4E-997A-3B472EC9065D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12196,8 +12206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14418,7 +14428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6:J7"/>
     </sheetView>
   </sheetViews>
@@ -14831,7 +14841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AE1005"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
+    <sheetView topLeftCell="X1" workbookViewId="0">
       <selection activeCell="AD6" sqref="AD6:AD1005"/>
     </sheetView>
   </sheetViews>
@@ -90726,7 +90736,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AP5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
renamed worksheet 'Sequence files' -> 'Sequence file'
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/current/filled/glioblastoma_1000cells.xlsx
+++ b/examples/spreadsheets/current/filled/glioblastoma_1000cells.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rolando/development/hca/metadata-schema/examples/spreadsheets/current/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{972BE2C4-79AE-C644-90BD-CA5CF7724D81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C1EA263E-DA7D-2247-BA29-94D68D353D62}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-10800" windowWidth="51200" windowHeight="28800" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-10800" windowWidth="51200" windowHeight="28800" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Donor organism" sheetId="4" r:id="rId4"/>
     <sheet name="Specimen from organism" sheetId="5" r:id="rId5"/>
     <sheet name="Cell suspension" sheetId="6" r:id="rId6"/>
-    <sheet name="Sequence files" sheetId="7" r:id="rId7"/>
+    <sheet name="Sequence file" sheetId="7" r:id="rId7"/>
     <sheet name="Organoid" sheetId="8" r:id="rId8"/>
     <sheet name="Collection protocol" sheetId="10" r:id="rId9"/>
     <sheet name="Dissociation protocol" sheetId="11" r:id="rId10"/>
@@ -40844,8 +40844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P2005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -90390,7 +90390,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>